<commit_message>
Added hydro one scanning method
</commit_message>
<xml_diff>
--- a/Funding Requested.xlsx
+++ b/Funding Requested.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LiBo3\PycharmProjects\PythonProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F0B8EC-4149-41D6-97E7-0A35E4AF51D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C323DA8-A27B-4DCE-9B09-73451014339F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -349,7 +349,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="A2:C3"/>
+      <selection activeCell="C4" sqref="A2:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>